<commit_message>
Added Throughput excel for `exp-46`
</commit_message>
<xml_diff>
--- a/Results/experiment-46-self-benchmark-GOPS-mul-multi-batch-square-sizes-fixed-iterations-raspberry-pi-4/throughput.xlsx
+++ b/Results/experiment-46-self-benchmark-GOPS-mul-multi-batch-square-sizes-fixed-iterations-raspberry-pi-4/throughput.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Size</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">(Int8-SelfDependentW4A4) / Int8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Int8-SelfDependentW4A4</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -900,11 +903,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="40296095"/>
-        <c:axId val="42353148"/>
+        <c:axId val="80218792"/>
+        <c:axId val="84604185"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40296095"/>
+        <c:axId val="80218792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,7 +972,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42353148"/>
+        <c:crossAx val="84604185"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -977,7 +980,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42353148"/>
+        <c:axId val="84604185"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1042,7 +1045,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40296095"/>
+        <c:crossAx val="80218792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1100,8 +1103,8 @@
       <xdr:rowOff>37800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19800</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2230560</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>172080</xdr:rowOff>
     </xdr:to>
@@ -1112,7 +1115,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="98640" y="2021040"/>
-        <a:ext cx="11584080" cy="5422320"/>
+        <a:ext cx="11530440" cy="5422320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1130,10 +1133,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1144,7 +1147,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="46.4"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1169,6 +1173,9 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -1193,6 +1200,10 @@
         <f aca="false">ROUND(((F2-B2)/B2)*100,2)</f>
         <v>191.25</v>
       </c>
+      <c r="H2" s="1" t="n">
+        <f aca="false">ROUND(F2-B2,2)</f>
+        <v>2.54</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -1217,6 +1228,10 @@
         <f aca="false">ROUND(((F3-B3)/B3)*100,2)</f>
         <v>81.93</v>
       </c>
+      <c r="H3" s="1" t="n">
+        <f aca="false">ROUND(F3-B3,2)</f>
+        <v>3.86</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -1241,6 +1256,10 @@
         <f aca="false">ROUND(((F4-B4)/B4)*100,2)</f>
         <v>57.16</v>
       </c>
+      <c r="H4" s="1" t="n">
+        <f aca="false">ROUND(F4-B4,2)</f>
+        <v>4.89</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -1265,6 +1284,10 @@
         <f aca="false">ROUND(((F5-B5)/B5)*100,2)</f>
         <v>40.34</v>
       </c>
+      <c r="H5" s="1" t="n">
+        <f aca="false">ROUND(F5-B5,2)</f>
+        <v>4.69</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -1289,6 +1312,10 @@
         <f aca="false">ROUND(((F6-B6)/B6)*100,2)</f>
         <v>12.51</v>
       </c>
+      <c r="H6" s="1" t="n">
+        <f aca="false">ROUND(F6-B6,2)</f>
+        <v>1.77</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -1313,6 +1340,10 @@
         <f aca="false">ROUND(((F7-B7)/B7)*100,2)</f>
         <v>11.36</v>
       </c>
+      <c r="H7" s="1" t="n">
+        <f aca="false">ROUND(F7-B7,2)</f>
+        <v>1.82</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -1337,6 +1368,10 @@
         <f aca="false">ROUND(((F8-B8)/B8)*100,2)</f>
         <v>8.43</v>
       </c>
+      <c r="H8" s="1" t="n">
+        <f aca="false">ROUND(F8-B8,2)</f>
+        <v>1.42</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -1360,6 +1395,10 @@
       <c r="G9" s="1" t="n">
         <f aca="false">ROUND(((F9-B9)/B9)*100,2)</f>
         <v>11.65</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <f aca="false">ROUND(F9-B9,2)</f>
+        <v>1.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>